<commit_message>
Update tables for GREAT results
</commit_message>
<xml_diff>
--- a/genomic_range/results/Precision_Table.xlsx
+++ b/genomic_range/results/Precision_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mei/Desktop/benchmarks/genomic_range/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajni\Desktop\benchmarks\genomic_range\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD59865-091F-654E-954C-7252349720AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E174B51-2020-4505-9BC6-07D022340177}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="16140" windowHeight="26780" xr2:uid="{9FDEA6EF-D5C4-7F45-96BD-DB608973E662}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9FDEA6EF-D5C4-7F45-96BD-DB608973E662}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Chipenrich_Colorectal_Cancer</t>
   </si>
@@ -43,327 +43,6 @@
   </si>
   <si>
     <t>Chipenrich_Prostate_Cancer</t>
-  </si>
-  <si>
-    <t>Sample</t>
-  </si>
-  <si>
-    <t>GSM1847178</t>
-  </si>
-  <si>
-    <t>GSE84618</t>
-  </si>
-  <si>
-    <t>GSM2283764</t>
-  </si>
-  <si>
-    <t>GSM2283765</t>
-  </si>
-  <si>
-    <t>GSM2283766</t>
-  </si>
-  <si>
-    <t>GSM2283767</t>
-  </si>
-  <si>
-    <t>GSM2283768</t>
-  </si>
-  <si>
-    <t>GSM2283769</t>
-  </si>
-  <si>
-    <t>GSM2283770</t>
-  </si>
-  <si>
-    <t>GSM2283771</t>
-  </si>
-  <si>
-    <t>GSM2283772</t>
-  </si>
-  <si>
-    <t>GSM2283773</t>
-  </si>
-  <si>
-    <t>GSM2283774</t>
-  </si>
-  <si>
-    <t>GSM2283775</t>
-  </si>
-  <si>
-    <t>GSM2101436</t>
-  </si>
-  <si>
-    <t>GSM2101437</t>
-  </si>
-  <si>
-    <t>GSM2752893</t>
-  </si>
-  <si>
-    <t>GSM2101438</t>
-  </si>
-  <si>
-    <t>GSM2101439</t>
-  </si>
-  <si>
-    <t>GSM2752894</t>
-  </si>
-  <si>
-    <t>GSM2752897</t>
-  </si>
-  <si>
-    <t>GSM2752898</t>
-  </si>
-  <si>
-    <t>GSM2752899</t>
-  </si>
-  <si>
-    <t>GSM2752900</t>
-  </si>
-  <si>
-    <t>GSM2752901</t>
-  </si>
-  <si>
-    <t>GSM2752895</t>
-  </si>
-  <si>
-    <t>GSM2298950</t>
-  </si>
-  <si>
-    <t>GSM2058015</t>
-  </si>
-  <si>
-    <t>GSM2058016</t>
-  </si>
-  <si>
-    <t>GSM2058017</t>
-  </si>
-  <si>
-    <t>GSM2058018</t>
-  </si>
-  <si>
-    <t>GSM2058019</t>
-  </si>
-  <si>
-    <t>GSM2058020</t>
-  </si>
-  <si>
-    <t>GSM2058021</t>
-  </si>
-  <si>
-    <t>GSM2058022</t>
-  </si>
-  <si>
-    <t>GSM2058023</t>
-  </si>
-  <si>
-    <t>GSM2058024</t>
-  </si>
-  <si>
-    <t>GSM2058025</t>
-  </si>
-  <si>
-    <t>GSM2058026</t>
-  </si>
-  <si>
-    <t>GSM2058027</t>
-  </si>
-  <si>
-    <t>GSM2058028</t>
-  </si>
-  <si>
-    <t>GSM2058029</t>
-  </si>
-  <si>
-    <t>GSM2058030</t>
-  </si>
-  <si>
-    <t>GSM2058031</t>
-  </si>
-  <si>
-    <t>GSM2058032</t>
-  </si>
-  <si>
-    <t>GSM2058033</t>
-  </si>
-  <si>
-    <t>GSM2058034</t>
-  </si>
-  <si>
-    <t>GSM2058035</t>
-  </si>
-  <si>
-    <t>GSM2058036</t>
-  </si>
-  <si>
-    <t>GSM2058037</t>
-  </si>
-  <si>
-    <t>GSM2058038</t>
-  </si>
-  <si>
-    <t>GSM2058039</t>
-  </si>
-  <si>
-    <t>GSM2058040</t>
-  </si>
-  <si>
-    <t>GSM2058041</t>
-  </si>
-  <si>
-    <t>GSM2058042</t>
-  </si>
-  <si>
-    <t>GSM2058043</t>
-  </si>
-  <si>
-    <t>GSM2058044</t>
-  </si>
-  <si>
-    <t>GSM2058045</t>
-  </si>
-  <si>
-    <t>GSM2058046</t>
-  </si>
-  <si>
-    <t>GSM2058047</t>
-  </si>
-  <si>
-    <t>GSM2058048</t>
-  </si>
-  <si>
-    <t>GSM2058049</t>
-  </si>
-  <si>
-    <t>GSM2058050</t>
-  </si>
-  <si>
-    <t>GSM2058051</t>
-  </si>
-  <si>
-    <t>GSM2058052</t>
-  </si>
-  <si>
-    <t>GSM2058053</t>
-  </si>
-  <si>
-    <t>GSM2058054</t>
-  </si>
-  <si>
-    <t>GSM2058055</t>
-  </si>
-  <si>
-    <t>GSM2058056</t>
-  </si>
-  <si>
-    <t>GSM2058057</t>
-  </si>
-  <si>
-    <t>GSM2058058</t>
-  </si>
-  <si>
-    <t>GSM2058059</t>
-  </si>
-  <si>
-    <t>GSM2058060</t>
-  </si>
-  <si>
-    <t>GSM2058061</t>
-  </si>
-  <si>
-    <t>GSM2058062</t>
-  </si>
-  <si>
-    <t>GSM2058063</t>
-  </si>
-  <si>
-    <t>GSM2058064</t>
-  </si>
-  <si>
-    <t>GSM2058065</t>
-  </si>
-  <si>
-    <t>GSM2058066</t>
-  </si>
-  <si>
-    <t>GSM2058067</t>
-  </si>
-  <si>
-    <t>GSM2058068</t>
-  </si>
-  <si>
-    <t>GSM2058069</t>
-  </si>
-  <si>
-    <t>GSM2058070</t>
-  </si>
-  <si>
-    <t>GSM2058071</t>
-  </si>
-  <si>
-    <t>GSM2058072</t>
-  </si>
-  <si>
-    <t>GSM2058073</t>
-  </si>
-  <si>
-    <t>GSM2058074</t>
-  </si>
-  <si>
-    <t>GSM2058075</t>
-  </si>
-  <si>
-    <t>GSM2058076</t>
-  </si>
-  <si>
-    <t>GSM2058077</t>
-  </si>
-  <si>
-    <t>GSM2058078</t>
-  </si>
-  <si>
-    <t>GSM2058079</t>
-  </si>
-  <si>
-    <t>GSM2058080</t>
-  </si>
-  <si>
-    <t>GSM2058081</t>
-  </si>
-  <si>
-    <t>GSM2058082</t>
-  </si>
-  <si>
-    <t>GSM2058083</t>
-  </si>
-  <si>
-    <t>GSM2058084</t>
-  </si>
-  <si>
-    <t>GSM2058085</t>
-  </si>
-  <si>
-    <t>GSM2058086</t>
-  </si>
-  <si>
-    <t>GSM2058087</t>
-  </si>
-  <si>
-    <t>GSM2058088</t>
-  </si>
-  <si>
-    <t>GSM2058089</t>
-  </si>
-  <si>
-    <t>GSM2058090</t>
-  </si>
-  <si>
-    <t>GSM2058091</t>
-  </si>
-  <si>
-    <t>GSM2058092</t>
-  </si>
-  <si>
-    <t>GSM2058093</t>
   </si>
   <si>
     <t>Chipenrich_Median_Precision</t>
@@ -433,7 +112,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -475,10 +154,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -793,43 +475,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DBC195-AB1D-C14E-9476-031E2CC25C6F}">
-  <dimension ref="A1:Z107"/>
+  <dimension ref="A1:Y107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2:Z107"/>
+    <sheetView tabSelected="1" topLeftCell="S91" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="U105" sqref="U105:X105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.625" customWidth="1"/>
+    <col min="2" max="2" width="27.625" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="24.625" customWidth="1"/>
     <col min="6" max="6" width="26.5" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" customWidth="1"/>
+    <col min="7" max="7" width="29.625" customWidth="1"/>
     <col min="8" max="8" width="23.5" customWidth="1"/>
     <col min="9" max="9" width="24.5" customWidth="1"/>
-    <col min="10" max="10" width="26.6640625" customWidth="1"/>
+    <col min="10" max="10" width="26.625" customWidth="1"/>
     <col min="11" max="11" width="28" customWidth="1"/>
-    <col min="12" max="12" width="30.83203125" customWidth="1"/>
-    <col min="13" max="13" width="25.83203125" customWidth="1"/>
-    <col min="14" max="14" width="26.83203125" customWidth="1"/>
+    <col min="12" max="12" width="30.875" customWidth="1"/>
+    <col min="13" max="13" width="25.875" customWidth="1"/>
+    <col min="14" max="14" width="26.875" customWidth="1"/>
     <col min="15" max="15" width="27.5" customWidth="1"/>
-    <col min="16" max="16" width="22.1640625" customWidth="1"/>
-    <col min="17" max="17" width="24.1640625" customWidth="1"/>
-    <col min="18" max="18" width="20.33203125" customWidth="1"/>
-    <col min="19" max="19" width="20.83203125" customWidth="1"/>
+    <col min="16" max="16" width="22.125" customWidth="1"/>
+    <col min="17" max="17" width="24.125" customWidth="1"/>
+    <col min="18" max="18" width="20.375" customWidth="1"/>
+    <col min="19" max="19" width="20.875" customWidth="1"/>
     <col min="20" max="20" width="23" customWidth="1"/>
-    <col min="21" max="21" width="12.5" customWidth="1"/>
-    <col min="22" max="22" width="20.5" customWidth="1"/>
-    <col min="23" max="23" width="18.33203125" customWidth="1"/>
-    <col min="24" max="24" width="18" customWidth="1"/>
-    <col min="25" max="25" width="17.6640625" customWidth="1"/>
-    <col min="26" max="26" width="20.5" customWidth="1"/>
+    <col min="21" max="21" width="20.5" customWidth="1"/>
+    <col min="22" max="22" width="18.375" customWidth="1"/>
+    <col min="23" max="23" width="18" customWidth="1"/>
+    <col min="24" max="24" width="17.625" customWidth="1"/>
+    <col min="25" max="25" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -843,73 +524,70 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>111</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>112</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>113</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>115</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>118</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>119</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>121</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>122</v>
+        <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>123</v>
+        <v>16</v>
       </c>
       <c r="R1" t="s">
-        <v>124</v>
+        <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>125</v>
+        <v>18</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="V1" t="s">
-        <v>127</v>
+        <v>21</v>
       </c>
       <c r="W1" t="s">
-        <v>128</v>
-      </c>
-      <c r="X1" t="s">
-        <v>129</v>
+        <v>22</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
       <c r="A2" s="1">
         <v>0.39100679999999999</v>
       </c>
@@ -974,15 +652,24 @@
         <f>MEDIAN($P2,$Q2,$R2,$S2)</f>
         <v>0</v>
       </c>
-      <c r="U2" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z2" t="e">
-        <f>MEDIAN($V2,$W2,$X2,$Y2)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <f>MEDIAN($U2,$V2,$W2,$X2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
       <c r="A3" s="1">
         <v>0.49751240000000002</v>
       </c>
@@ -1047,15 +734,24 @@
         <f t="shared" ref="T3:T66" si="3">MEDIAN($P3,$Q3,$R3,$S3)</f>
         <v>0</v>
       </c>
-      <c r="U3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z3" t="e">
-        <f t="shared" ref="Z3:Z66" si="4">MEDIAN($V3,$W3,$X3,$Y3)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="U3">
+        <v>3.7037040000000001</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" ref="Y3:Y66" si="4">MEDIAN($U3,$V3,$W3,$X3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
       <c r="A4" s="1">
         <v>0.42265429999999998</v>
       </c>
@@ -1104,72 +800,78 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U4" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z4" t="e">
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y5" t="e">
         <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U5" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z5" t="e">
-        <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25">
       <c r="A6" s="1">
         <v>0.42301179999999999</v>
       </c>
@@ -1218,15 +920,24 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z6" t="e">
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
       <c r="A7" s="1">
         <v>0.7042254</v>
       </c>
@@ -1275,15 +986,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U7" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z7" t="e">
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
       <c r="A8" s="1">
         <v>0.31347960000000002</v>
       </c>
@@ -1348,15 +1068,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U8" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z8" t="e">
+      <c r="U8" s="1">
+        <v>0</v>
+      </c>
+      <c r="V8" s="1">
+        <v>0</v>
+      </c>
+      <c r="W8" s="1">
+        <v>0</v>
+      </c>
+      <c r="X8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y8">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
       <c r="A9" s="1">
         <v>0.31347960000000002</v>
       </c>
@@ -1421,15 +1150,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U9" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z9" t="e">
+      <c r="U9" s="1">
+        <v>0</v>
+      </c>
+      <c r="V9" s="1">
+        <v>0</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0</v>
+      </c>
+      <c r="X9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y9">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
       <c r="A10" s="1">
         <v>0.31347960000000002</v>
       </c>
@@ -1494,15 +1232,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U10" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z10" t="e">
+      <c r="U10" s="1">
+        <v>0</v>
+      </c>
+      <c r="V10" s="1">
+        <v>0</v>
+      </c>
+      <c r="W10" s="1">
+        <v>0</v>
+      </c>
+      <c r="X10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y10">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
       <c r="A11" s="1">
         <v>0.31347960000000002</v>
       </c>
@@ -1567,15 +1314,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U11" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z11" t="e">
+      <c r="U11" s="3">
+        <v>0</v>
+      </c>
+      <c r="V11" s="3">
+        <v>0</v>
+      </c>
+      <c r="W11" s="3">
+        <v>0</v>
+      </c>
+      <c r="X11" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y11">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
       <c r="A12" s="1">
         <v>0.37878790000000001</v>
       </c>
@@ -1624,15 +1380,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U12" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z12" t="e">
+      <c r="U12" s="4">
+        <v>0</v>
+      </c>
+      <c r="V12" s="4">
+        <v>0</v>
+      </c>
+      <c r="W12" s="4">
+        <v>0</v>
+      </c>
+      <c r="X12" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y12">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
       <c r="A13" s="1">
         <v>0.45696880000000001</v>
       </c>
@@ -1697,15 +1462,24 @@
         <f t="shared" si="3"/>
         <v>0.72463770000000005</v>
       </c>
-      <c r="U13" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z13" t="e">
+      <c r="U13" s="5">
+        <v>0</v>
+      </c>
+      <c r="V13" s="5">
+        <v>0</v>
+      </c>
+      <c r="W13" s="5">
+        <v>0</v>
+      </c>
+      <c r="X13" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y13">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
       <c r="A14" s="1">
         <v>0.45696880000000001</v>
       </c>
@@ -1770,15 +1544,16 @@
         <f t="shared" si="3"/>
         <v>0.72463770000000005</v>
       </c>
-      <c r="U14" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z14" t="e">
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" t="e">
         <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25">
       <c r="A15" s="1">
         <v>0.45696880000000001</v>
       </c>
@@ -1843,15 +1618,24 @@
         <f t="shared" si="3"/>
         <v>0.72463770000000005</v>
       </c>
-      <c r="U15" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z15" t="e">
+      <c r="U15" s="5">
+        <v>0</v>
+      </c>
+      <c r="V15" s="5">
+        <v>0</v>
+      </c>
+      <c r="W15" s="5">
+        <v>0</v>
+      </c>
+      <c r="X15" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y15">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
       <c r="A16" s="1">
         <v>0.3289474</v>
       </c>
@@ -1916,15 +1700,16 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U16" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z16" t="e">
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" t="e">
         <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25">
       <c r="A17" s="1">
         <v>0.46317740000000002</v>
       </c>
@@ -1989,15 +1774,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U17" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z17" t="e">
+      <c r="U17" s="5">
+        <v>0</v>
+      </c>
+      <c r="V17" s="5">
+        <v>0</v>
+      </c>
+      <c r="W17" s="5">
+        <v>0</v>
+      </c>
+      <c r="X17" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y17">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25">
       <c r="A18" s="1">
         <v>0.540906</v>
       </c>
@@ -2046,15 +1840,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U18" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z18" t="e">
+      <c r="Y18" t="e">
         <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25">
       <c r="A19" s="1">
         <v>0.55865920000000002</v>
       </c>
@@ -2119,15 +1910,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U19" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z19" t="e">
+      <c r="U19" s="5">
+        <v>0</v>
+      </c>
+      <c r="V19" s="5">
+        <v>0</v>
+      </c>
+      <c r="W19" s="5">
+        <v>0</v>
+      </c>
+      <c r="X19" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y19">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25">
       <c r="A20" s="1">
         <v>0.28409089999999998</v>
       </c>
@@ -2192,15 +1992,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U20" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z20" t="e">
+      <c r="U20" s="5">
+        <v>0</v>
+      </c>
+      <c r="V20" s="5">
+        <v>0</v>
+      </c>
+      <c r="W20" s="5">
+        <v>0</v>
+      </c>
+      <c r="X20" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y20">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25">
       <c r="A21" s="1">
         <v>0.26281209999999999</v>
       </c>
@@ -2249,15 +2058,24 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U21" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z21" t="e">
+      <c r="U21" s="5">
+        <v>0</v>
+      </c>
+      <c r="V21" s="5">
+        <v>0</v>
+      </c>
+      <c r="W21" s="5">
+        <v>0</v>
+      </c>
+      <c r="X21" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y21">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25">
       <c r="A22" s="1">
         <v>0.1644737</v>
       </c>
@@ -2322,15 +2140,24 @@
         <f t="shared" si="3"/>
         <v>0.67816094999999998</v>
       </c>
-      <c r="U22" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z22" t="e">
+      <c r="U22" s="5">
+        <v>0</v>
+      </c>
+      <c r="V22" s="5">
+        <v>0</v>
+      </c>
+      <c r="W22" s="5">
+        <v>0</v>
+      </c>
+      <c r="X22" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y22">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25">
       <c r="A23" s="1">
         <v>0.45180720000000002</v>
       </c>
@@ -2392,15 +2219,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U23" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z23" t="e">
+      <c r="U23" s="5">
+        <v>0</v>
+      </c>
+      <c r="V23" s="5">
+        <v>0</v>
+      </c>
+      <c r="W23" s="5">
+        <v>0</v>
+      </c>
+      <c r="X23" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y23">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25">
       <c r="A24" s="1">
         <v>9.5328880000000005E-2</v>
       </c>
@@ -2449,15 +2285,24 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U24" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z24" t="e">
+      <c r="U24" s="5">
+        <v>0</v>
+      </c>
+      <c r="V24" s="5">
+        <v>0</v>
+      </c>
+      <c r="W24" s="5">
+        <v>0</v>
+      </c>
+      <c r="X24" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y24">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25">
       <c r="A25" s="1">
         <v>0.13054830000000001</v>
       </c>
@@ -2506,15 +2351,24 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U25" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z25" t="e">
+      <c r="U25" s="5">
+        <v>0</v>
+      </c>
+      <c r="V25" s="5">
+        <v>0</v>
+      </c>
+      <c r="W25" s="5">
+        <v>0</v>
+      </c>
+      <c r="X25" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y25">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25">
       <c r="A26" s="1">
         <v>0.63124670000000005</v>
       </c>
@@ -2563,15 +2417,24 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U26" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z26" t="e">
+      <c r="U26" s="5">
+        <v>0</v>
+      </c>
+      <c r="V26" s="5">
+        <v>0</v>
+      </c>
+      <c r="W26" s="5">
+        <v>0</v>
+      </c>
+      <c r="X26" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y26">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25">
       <c r="A27" s="1">
         <v>0.57703400000000005</v>
       </c>
@@ -2636,15 +2499,24 @@
         <f t="shared" si="3"/>
         <v>0.76375934999999995</v>
       </c>
-      <c r="U27" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z27" t="e">
+      <c r="U27" s="5">
+        <v>0</v>
+      </c>
+      <c r="V27" s="5">
+        <v>0</v>
+      </c>
+      <c r="W27" s="5">
+        <v>0</v>
+      </c>
+      <c r="X27" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y27">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25">
       <c r="A28" s="1">
         <v>0.20661160000000001</v>
       </c>
@@ -2709,15 +2581,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U28" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z28" t="e">
+      <c r="U28" s="5">
+        <v>0</v>
+      </c>
+      <c r="V28" s="5">
+        <v>0</v>
+      </c>
+      <c r="W28" s="5">
+        <v>0</v>
+      </c>
+      <c r="X28" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y28">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25">
       <c r="A29" s="1">
         <v>0.3956479</v>
       </c>
@@ -2782,15 +2663,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U29" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z29" t="e">
+      <c r="Y29" t="e">
         <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25">
       <c r="A30" s="1">
         <v>0.60362170000000004</v>
       </c>
@@ -2855,15 +2733,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U30" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z30" t="e">
+      <c r="U30" s="5">
+        <v>0</v>
+      </c>
+      <c r="V30" s="5">
+        <v>0</v>
+      </c>
+      <c r="W30" s="5">
+        <v>0</v>
+      </c>
+      <c r="X30" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y30">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25">
       <c r="A31" s="1">
         <v>0.41562759999999999</v>
       </c>
@@ -2928,15 +2815,12 @@
         <f t="shared" si="3"/>
         <v>2.2916664999999998</v>
       </c>
-      <c r="U31" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z31" t="e">
+      <c r="Y31" t="e">
         <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25">
       <c r="A32" s="1">
         <v>0.48923680000000003</v>
       </c>
@@ -3001,15 +2885,12 @@
         <f t="shared" si="3"/>
         <v>1.7592595</v>
       </c>
-      <c r="U32" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z32" t="e">
+      <c r="Y32" t="e">
         <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25">
       <c r="A33" s="1">
         <v>0.127551</v>
       </c>
@@ -3074,15 +2955,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U33" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z33" t="e">
+      <c r="Y33" t="e">
         <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25">
       <c r="A34" s="1">
         <v>0.40160639999999997</v>
       </c>
@@ -3147,15 +3025,12 @@
         <f t="shared" si="3"/>
         <v>1.8853955</v>
       </c>
-      <c r="U34" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z34" t="e">
+      <c r="Y34" t="e">
         <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25">
       <c r="A35" s="1">
         <v>0.47647410000000001</v>
       </c>
@@ -3220,15 +3095,24 @@
         <f t="shared" si="3"/>
         <v>1.3022155</v>
       </c>
-      <c r="U35" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z35" t="e">
+      <c r="U35" s="5">
+        <v>0</v>
+      </c>
+      <c r="V35" s="5">
+        <v>0</v>
+      </c>
+      <c r="W35" s="5">
+        <v>0</v>
+      </c>
+      <c r="X35" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y35">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25">
       <c r="A36" s="1">
         <v>0.48701299999999997</v>
       </c>
@@ -3293,15 +3177,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U36" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z36" t="e">
+      <c r="U36" s="5">
+        <v>0</v>
+      </c>
+      <c r="V36" s="5">
+        <v>0</v>
+      </c>
+      <c r="W36" s="5">
+        <v>0</v>
+      </c>
+      <c r="X36" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y36">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25">
       <c r="A37" s="1">
         <v>0.56657219999999997</v>
       </c>
@@ -3366,15 +3259,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U37" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z37" t="e">
+      <c r="U37" s="5">
+        <v>0</v>
+      </c>
+      <c r="V37" s="5">
+        <v>0</v>
+      </c>
+      <c r="W37" s="5">
+        <v>0</v>
+      </c>
+      <c r="X37" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y37">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25">
       <c r="A38" s="1">
         <v>0.50111360000000005</v>
       </c>
@@ -3439,15 +3341,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U38" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z38" t="e">
+      <c r="U38" s="5">
+        <v>0</v>
+      </c>
+      <c r="V38" s="5">
+        <v>0</v>
+      </c>
+      <c r="W38" s="5">
+        <v>0</v>
+      </c>
+      <c r="X38" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y38">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25">
       <c r="A39" s="1">
         <v>0.52002079999999995</v>
       </c>
@@ -3512,15 +3423,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U39" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z39" t="e">
+      <c r="U39" s="5">
+        <v>0</v>
+      </c>
+      <c r="V39" s="5">
+        <v>0</v>
+      </c>
+      <c r="W39" s="5">
+        <v>0</v>
+      </c>
+      <c r="X39" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y39">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25">
       <c r="A40" s="1">
         <v>0.54282269999999999</v>
       </c>
@@ -3585,15 +3505,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U40" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z40" t="e">
+      <c r="U40" s="5">
+        <v>0</v>
+      </c>
+      <c r="V40" s="5">
+        <v>0</v>
+      </c>
+      <c r="W40" s="5">
+        <v>0</v>
+      </c>
+      <c r="X40" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y40">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25">
       <c r="A41" s="1">
         <v>0.54794520000000002</v>
       </c>
@@ -3658,15 +3587,24 @@
         <f t="shared" si="3"/>
         <v>0.70176305000000005</v>
       </c>
-      <c r="U41" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z41" t="e">
+      <c r="U41" s="5">
+        <v>0</v>
+      </c>
+      <c r="V41" s="5">
+        <v>0</v>
+      </c>
+      <c r="W41" s="5">
+        <v>0</v>
+      </c>
+      <c r="X41" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y41">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25">
       <c r="A42" s="1">
         <v>0.20523350000000001</v>
       </c>
@@ -3731,15 +3669,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U42" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z42" t="e">
+      <c r="U42" s="5">
+        <v>0</v>
+      </c>
+      <c r="V42" s="5">
+        <v>0</v>
+      </c>
+      <c r="W42" s="5">
+        <v>0</v>
+      </c>
+      <c r="X42" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y42">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25">
       <c r="A43" s="1">
         <v>0.52562419999999999</v>
       </c>
@@ -3804,15 +3751,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U43" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z43" t="e">
+      <c r="U43" s="5">
+        <v>0</v>
+      </c>
+      <c r="V43" s="5">
+        <v>0</v>
+      </c>
+      <c r="W43" s="5">
+        <v>0</v>
+      </c>
+      <c r="X43" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y43">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25">
       <c r="A44" s="1">
         <v>0.45271630000000002</v>
       </c>
@@ -3877,15 +3833,24 @@
         <f t="shared" si="3"/>
         <v>0.51414219999999999</v>
       </c>
-      <c r="U44" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z44" t="e">
+      <c r="U44" s="5">
+        <v>0</v>
+      </c>
+      <c r="V44" s="5">
+        <v>0</v>
+      </c>
+      <c r="W44" s="5">
+        <v>0</v>
+      </c>
+      <c r="X44" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y44">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25">
       <c r="A45" s="1">
         <v>0.66926940000000001</v>
       </c>
@@ -3950,15 +3915,24 @@
         <f t="shared" si="3"/>
         <v>0.30303029999999997</v>
       </c>
-      <c r="U45" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z45" t="e">
+      <c r="U45" s="5">
+        <v>0</v>
+      </c>
+      <c r="V45" s="5">
+        <v>0</v>
+      </c>
+      <c r="W45" s="5">
+        <v>0</v>
+      </c>
+      <c r="X45" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y45">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25">
       <c r="A46" s="1">
         <v>0.58651030000000004</v>
       </c>
@@ -4023,15 +3997,12 @@
         <f t="shared" si="3"/>
         <v>0.53911884999999993</v>
       </c>
-      <c r="U46" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z46" t="e">
+      <c r="Y46" t="e">
         <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25">
       <c r="A47" s="1">
         <v>0.61996280000000004</v>
       </c>
@@ -4096,15 +4067,24 @@
         <f t="shared" si="3"/>
         <v>0.7785048</v>
       </c>
-      <c r="U47" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z47" t="e">
+      <c r="U47" s="5">
+        <v>0</v>
+      </c>
+      <c r="V47" s="5">
+        <v>0</v>
+      </c>
+      <c r="W47" s="5">
+        <v>0</v>
+      </c>
+      <c r="X47" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y47">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25">
       <c r="A48" s="1">
         <v>0.43124099999999999</v>
       </c>
@@ -4153,15 +4133,24 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U48" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z48" t="e">
+      <c r="U48" s="5">
+        <v>0</v>
+      </c>
+      <c r="V48" s="5">
+        <v>0</v>
+      </c>
+      <c r="W48" s="5">
+        <v>0</v>
+      </c>
+      <c r="X48" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y48">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25">
       <c r="A49" s="1">
         <v>0.49658600000000003</v>
       </c>
@@ -4210,15 +4199,24 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U49" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z49" t="e">
+      <c r="U49" s="5">
+        <v>0</v>
+      </c>
+      <c r="V49" s="5">
+        <v>0</v>
+      </c>
+      <c r="W49" s="5">
+        <v>0</v>
+      </c>
+      <c r="X49" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y49">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25">
       <c r="A50" s="1">
         <v>0.52840160000000003</v>
       </c>
@@ -4267,15 +4265,24 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U50" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z50" t="e">
+      <c r="U50" s="5">
+        <v>0</v>
+      </c>
+      <c r="V50" s="5">
+        <v>0</v>
+      </c>
+      <c r="W50" s="5">
+        <v>0</v>
+      </c>
+      <c r="X50" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y50">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25">
       <c r="A51" s="1">
         <v>0.49751240000000002</v>
       </c>
@@ -4340,15 +4347,24 @@
         <f t="shared" si="3"/>
         <v>1.8248175</v>
       </c>
-      <c r="U51" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z51" t="e">
+      <c r="U51" s="5">
+        <v>0</v>
+      </c>
+      <c r="V51" s="5">
+        <v>0</v>
+      </c>
+      <c r="W51" s="5">
+        <v>0</v>
+      </c>
+      <c r="X51" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y51">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25">
       <c r="A52" s="1">
         <v>0.49889139999999998</v>
       </c>
@@ -4413,15 +4429,24 @@
         <f t="shared" si="3"/>
         <v>0.77221230000000007</v>
       </c>
-      <c r="U52" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z52" t="e">
+      <c r="U52" s="5">
+        <v>0</v>
+      </c>
+      <c r="V52" s="5">
+        <v>0</v>
+      </c>
+      <c r="W52" s="5">
+        <v>0</v>
+      </c>
+      <c r="X52" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y52">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25">
       <c r="A53" s="1">
         <v>0.36182720000000002</v>
       </c>
@@ -4486,15 +4511,24 @@
         <f t="shared" si="3"/>
         <v>1.181875</v>
       </c>
-      <c r="U53" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z53" t="e">
+      <c r="U53" s="5">
+        <v>0</v>
+      </c>
+      <c r="V53" s="5">
+        <v>0</v>
+      </c>
+      <c r="W53" s="5">
+        <v>0</v>
+      </c>
+      <c r="X53" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y53">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25">
       <c r="A54" s="1">
         <v>0.60350029999999999</v>
       </c>
@@ -4559,15 +4593,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U54" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z54" t="e">
+      <c r="U54" s="5">
+        <v>0</v>
+      </c>
+      <c r="V54" s="5">
+        <v>0</v>
+      </c>
+      <c r="W54" s="5">
+        <v>0</v>
+      </c>
+      <c r="X54" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y54">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25">
       <c r="A55" s="1">
         <v>0.47361300000000001</v>
       </c>
@@ -4632,15 +4675,24 @@
         <f t="shared" si="3"/>
         <v>0.72735930000000004</v>
       </c>
-      <c r="U55" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z55" t="e">
+      <c r="U55" s="5">
+        <v>0</v>
+      </c>
+      <c r="V55" s="5">
+        <v>0</v>
+      </c>
+      <c r="W55" s="5">
+        <v>0</v>
+      </c>
+      <c r="X55" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y55">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25">
       <c r="A56" s="1">
         <v>0.52770450000000002</v>
       </c>
@@ -4705,15 +4757,24 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U56" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z56" t="e">
+      <c r="U56" s="5">
+        <v>0</v>
+      </c>
+      <c r="V56" s="5">
+        <v>0</v>
+      </c>
+      <c r="W56" s="5">
+        <v>0</v>
+      </c>
+      <c r="X56" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y56">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25">
       <c r="A57" s="1">
         <v>0.35242289999999998</v>
       </c>
@@ -4778,15 +4839,24 @@
         <f t="shared" si="3"/>
         <v>0.24390244999999999</v>
       </c>
-      <c r="U57" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z57" t="e">
+      <c r="U57" s="5">
+        <v>0</v>
+      </c>
+      <c r="V57" s="5">
+        <v>0</v>
+      </c>
+      <c r="W57" s="5">
+        <v>0</v>
+      </c>
+      <c r="X57" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y57">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25">
       <c r="A58" s="1">
         <v>0.61050059999999995</v>
       </c>
@@ -4851,15 +4921,24 @@
         <f t="shared" si="3"/>
         <v>0.32258065000000002</v>
       </c>
-      <c r="U58" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z58" t="e">
+      <c r="U58" s="5">
+        <v>0</v>
+      </c>
+      <c r="V58" s="5">
+        <v>0</v>
+      </c>
+      <c r="W58" s="5">
+        <v>0</v>
+      </c>
+      <c r="X58" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y58">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25">
       <c r="A59" s="1">
         <v>0.69356870000000004</v>
       </c>
@@ -4924,15 +5003,24 @@
         <f t="shared" si="3"/>
         <v>0.61737805000000001</v>
       </c>
-      <c r="U59" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z59" t="e">
+      <c r="U59" s="5">
+        <v>0</v>
+      </c>
+      <c r="V59" s="5">
+        <v>0</v>
+      </c>
+      <c r="W59" s="5">
+        <v>0</v>
+      </c>
+      <c r="X59" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y59">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25">
       <c r="A60" s="1">
         <v>0.54288820000000004</v>
       </c>
@@ -4997,15 +5085,24 @@
         <f t="shared" si="3"/>
         <v>0.58309529999999998</v>
       </c>
-      <c r="U60" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z60" t="e">
+      <c r="U60" s="5">
+        <v>0</v>
+      </c>
+      <c r="V60" s="5">
+        <v>0</v>
+      </c>
+      <c r="W60" s="5">
+        <v>0</v>
+      </c>
+      <c r="X60" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y60">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25">
       <c r="A61" s="1">
         <v>0.48997770000000002</v>
       </c>
@@ -5070,15 +5167,24 @@
         <f t="shared" si="3"/>
         <v>1.2886600000000001</v>
       </c>
-      <c r="U61" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z61" t="e">
+      <c r="U61" s="5">
+        <v>0</v>
+      </c>
+      <c r="V61" s="5">
+        <v>0</v>
+      </c>
+      <c r="W61" s="5">
+        <v>0</v>
+      </c>
+      <c r="X61" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y61">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25">
       <c r="A62" s="1">
         <v>0.42038890000000001</v>
       </c>
@@ -5143,15 +5249,24 @@
         <f t="shared" si="3"/>
         <v>1.4642854999999999</v>
       </c>
-      <c r="U62" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z62" t="e">
+      <c r="U62" s="5">
+        <v>0</v>
+      </c>
+      <c r="V62" s="5">
+        <v>0</v>
+      </c>
+      <c r="W62" s="5">
+        <v>0</v>
+      </c>
+      <c r="X62" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y62">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25">
       <c r="A63" s="1">
         <v>0.5347594</v>
       </c>
@@ -5216,15 +5331,24 @@
         <f t="shared" si="3"/>
         <v>0.67340829999999996</v>
       </c>
-      <c r="U63" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z63" t="e">
+      <c r="U63" s="5">
+        <v>0</v>
+      </c>
+      <c r="V63" s="5">
+        <v>0</v>
+      </c>
+      <c r="W63" s="5">
+        <v>0</v>
+      </c>
+      <c r="X63" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y63">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:25">
       <c r="A64" s="1">
         <v>0.34687810000000002</v>
       </c>
@@ -5289,15 +5413,24 @@
         <f t="shared" si="3"/>
         <v>0.82988980000000001</v>
       </c>
-      <c r="U64" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z64" t="e">
+      <c r="U64" s="5">
+        <v>0</v>
+      </c>
+      <c r="V64" s="5">
+        <v>0</v>
+      </c>
+      <c r="W64" s="5">
+        <v>0</v>
+      </c>
+      <c r="X64" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y64">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:25">
       <c r="A65" s="1">
         <v>0.30864200000000003</v>
       </c>
@@ -5362,15 +5495,24 @@
         <f t="shared" si="3"/>
         <v>0.59899570000000002</v>
       </c>
-      <c r="U65" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z65" t="e">
+      <c r="U65" s="5">
+        <v>0</v>
+      </c>
+      <c r="V65" s="5">
+        <v>0</v>
+      </c>
+      <c r="W65" s="5">
+        <v>0</v>
+      </c>
+      <c r="X65" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y65">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:25">
       <c r="A66" s="1">
         <v>0.34636319999999998</v>
       </c>
@@ -5435,15 +5577,24 @@
         <f t="shared" si="3"/>
         <v>0.71707619999999994</v>
       </c>
-      <c r="U66" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z66" t="e">
+      <c r="U66" s="5">
+        <v>0</v>
+      </c>
+      <c r="V66" s="5">
+        <v>0</v>
+      </c>
+      <c r="W66" s="5">
+        <v>0</v>
+      </c>
+      <c r="X66" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y66">
         <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:25">
       <c r="A67" s="1">
         <v>0.53050399999999998</v>
       </c>
@@ -5492,15 +5643,24 @@
         <f t="shared" ref="O67:O107" si="7">MEDIAN($K67,$L67,$M67,$N67)</f>
         <v>0</v>
       </c>
-      <c r="U67" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z67" t="e">
-        <f t="shared" ref="Z67:Z107" si="8">MEDIAN($V67,$W67,$X67,$Y67)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="U67" s="5">
+        <v>0</v>
+      </c>
+      <c r="V67" s="5">
+        <v>0</v>
+      </c>
+      <c r="W67" s="5">
+        <v>0</v>
+      </c>
+      <c r="X67" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y67">
+        <f t="shared" ref="Y67:Y107" si="8">MEDIAN($U67,$V67,$W67,$X67)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25">
       <c r="A68" s="1">
         <v>0.47460839999999999</v>
       </c>
@@ -5565,15 +5725,24 @@
         <f t="shared" ref="T68:T107" si="9">MEDIAN($P68,$Q68,$R68,$S68)</f>
         <v>1.0025124999999999</v>
       </c>
-      <c r="U68" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z68" t="e">
+      <c r="U68" s="5">
+        <v>0</v>
+      </c>
+      <c r="V68" s="5">
+        <v>0</v>
+      </c>
+      <c r="W68" s="5">
+        <v>0</v>
+      </c>
+      <c r="X68" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y68">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25">
       <c r="A69" s="1">
         <v>0.37373200000000001</v>
       </c>
@@ -5638,15 +5807,24 @@
         <f t="shared" si="9"/>
         <v>0.83023285000000002</v>
       </c>
-      <c r="U69" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z69" t="e">
+      <c r="U69" s="5">
+        <v>0</v>
+      </c>
+      <c r="V69" s="5">
+        <v>0</v>
+      </c>
+      <c r="W69" s="5">
+        <v>0</v>
+      </c>
+      <c r="X69" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y69">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:25">
       <c r="A70" s="1">
         <v>0.5569307</v>
       </c>
@@ -5711,15 +5889,12 @@
         <f t="shared" si="9"/>
         <v>0.76099534999999996</v>
       </c>
-      <c r="U70" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z70" t="e">
+      <c r="Y70" t="e">
         <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:25">
       <c r="A71" s="1">
         <v>0.23909150000000001</v>
       </c>
@@ -5784,15 +5959,24 @@
         <f t="shared" si="9"/>
         <v>0.30674845000000001</v>
       </c>
-      <c r="U71" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z71" t="e">
+      <c r="U71" s="5">
+        <v>0</v>
+      </c>
+      <c r="V71" s="5">
+        <v>0</v>
+      </c>
+      <c r="W71" s="5">
+        <v>0</v>
+      </c>
+      <c r="X71" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y71">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:25">
       <c r="A72" s="1">
         <v>0.28037380000000001</v>
       </c>
@@ -5857,15 +6041,24 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U72" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z72" t="e">
+      <c r="U72" s="5">
+        <v>0</v>
+      </c>
+      <c r="V72" s="5">
+        <v>0</v>
+      </c>
+      <c r="W72" s="5">
+        <v>0</v>
+      </c>
+      <c r="X72" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y72">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:25">
       <c r="A73" s="1">
         <v>0.41987400000000002</v>
       </c>
@@ -5930,15 +6123,12 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U73" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z73" t="e">
+      <c r="Y73" t="e">
         <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:25">
       <c r="A74" s="1">
         <v>0.7175473</v>
       </c>
@@ -6003,15 +6193,24 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U74" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z74" t="e">
+      <c r="U74" s="5">
+        <v>0</v>
+      </c>
+      <c r="V74" s="5">
+        <v>0</v>
+      </c>
+      <c r="W74" s="5">
+        <v>0</v>
+      </c>
+      <c r="X74" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y74">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:25">
       <c r="A75" s="1">
         <v>0.39904230000000002</v>
       </c>
@@ -6076,15 +6275,12 @@
         <f t="shared" si="9"/>
         <v>0.50505049999999996</v>
       </c>
-      <c r="U75" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z75" t="e">
+      <c r="Y75" t="e">
         <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:25">
       <c r="A76" s="1">
         <v>0.43699929999999998</v>
       </c>
@@ -6149,15 +6345,12 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U76" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z76" t="e">
+      <c r="Y76" t="e">
         <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:25">
       <c r="A77" s="1">
         <v>0.55594160000000004</v>
       </c>
@@ -6222,15 +6415,24 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U77" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z77" t="e">
+      <c r="U77" s="5">
+        <v>0</v>
+      </c>
+      <c r="V77" s="5">
+        <v>0</v>
+      </c>
+      <c r="W77" s="5">
+        <v>0</v>
+      </c>
+      <c r="X77" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y77">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:25">
       <c r="A78" s="1">
         <v>0.49046319999999999</v>
       </c>
@@ -6295,15 +6497,24 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U78" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z78" t="e">
+      <c r="U78" s="5">
+        <v>0</v>
+      </c>
+      <c r="V78" s="5">
+        <v>0</v>
+      </c>
+      <c r="W78" s="5">
+        <v>0</v>
+      </c>
+      <c r="X78" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y78">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:25">
       <c r="A79" s="1">
         <v>0.46419100000000002</v>
       </c>
@@ -6368,15 +6579,24 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U79" t="s">
-        <v>82</v>
-      </c>
-      <c r="Z79" t="e">
+      <c r="U79" s="5">
+        <v>0</v>
+      </c>
+      <c r="V79" s="5">
+        <v>0</v>
+      </c>
+      <c r="W79" s="5">
+        <v>0</v>
+      </c>
+      <c r="X79" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y79">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:25">
       <c r="A80" s="1">
         <v>0.44286979999999998</v>
       </c>
@@ -6441,15 +6661,12 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U80" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z80" t="e">
+      <c r="Y80" t="e">
         <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:25">
       <c r="A81" s="1">
         <v>0.55970149999999996</v>
       </c>
@@ -6514,15 +6731,12 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U81" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z81" t="e">
+      <c r="Y81" t="e">
         <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:25">
       <c r="A82" s="1">
         <v>0.60422960000000003</v>
       </c>
@@ -6587,15 +6801,24 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U82" t="s">
-        <v>85</v>
-      </c>
-      <c r="Z82" t="e">
+      <c r="U82" s="5">
+        <v>0</v>
+      </c>
+      <c r="V82" s="5">
+        <v>0</v>
+      </c>
+      <c r="W82" s="5">
+        <v>0</v>
+      </c>
+      <c r="X82" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y82">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:25">
       <c r="A83" s="1">
         <v>0.36023050000000001</v>
       </c>
@@ -6660,15 +6883,24 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U83" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z83" t="e">
+      <c r="U83" s="5">
+        <v>0</v>
+      </c>
+      <c r="V83" s="5">
+        <v>0</v>
+      </c>
+      <c r="W83" s="5">
+        <v>0</v>
+      </c>
+      <c r="X83" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y83">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:25">
       <c r="A84" s="1">
         <v>0.41736230000000002</v>
       </c>
@@ -6733,15 +6965,12 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U84" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z84" t="e">
+      <c r="Y84" t="e">
         <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:25">
       <c r="A85" s="1">
         <v>0.37509379999999998</v>
       </c>
@@ -6806,15 +7035,24 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U85" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z85" t="e">
+      <c r="U85" s="5">
+        <v>0</v>
+      </c>
+      <c r="V85" s="5">
+        <v>0</v>
+      </c>
+      <c r="W85" s="5">
+        <v>0</v>
+      </c>
+      <c r="X85" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y85">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:25">
       <c r="A86" s="1">
         <v>0.2735978</v>
       </c>
@@ -6879,15 +7117,24 @@
         <f t="shared" si="9"/>
         <v>0.54945049999999995</v>
       </c>
-      <c r="U86" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z86" t="e">
+      <c r="U86" s="5">
+        <v>0</v>
+      </c>
+      <c r="V86" s="5">
+        <v>0</v>
+      </c>
+      <c r="W86" s="5">
+        <v>0</v>
+      </c>
+      <c r="X86" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y86">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:25">
       <c r="A87" s="1">
         <v>0.247117</v>
       </c>
@@ -6952,15 +7199,12 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U87" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z87" t="e">
+      <c r="Y87" t="e">
         <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:25">
       <c r="A88" s="1">
         <v>0.34891840000000002</v>
       </c>
@@ -7025,15 +7269,24 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U88" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z88" t="e">
+      <c r="U88" s="5">
+        <v>0</v>
+      </c>
+      <c r="V88" s="5">
+        <v>0</v>
+      </c>
+      <c r="W88" s="5">
+        <v>0</v>
+      </c>
+      <c r="X88" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y88">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:25">
       <c r="A89" s="1">
         <v>0.29048659999999998</v>
       </c>
@@ -7098,15 +7351,24 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U89" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z89" t="e">
+      <c r="U89" s="5">
+        <v>0</v>
+      </c>
+      <c r="V89" s="5">
+        <v>0</v>
+      </c>
+      <c r="W89" s="5">
+        <v>0</v>
+      </c>
+      <c r="X89" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y89">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:25">
       <c r="A90" s="1">
         <v>0.35561880000000001</v>
       </c>
@@ -7171,15 +7433,24 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U90" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z90" t="e">
+      <c r="U90" s="5">
+        <v>0</v>
+      </c>
+      <c r="V90" s="5">
+        <v>0</v>
+      </c>
+      <c r="W90" s="5">
+        <v>0</v>
+      </c>
+      <c r="X90" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y90">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:25">
       <c r="A91" s="1">
         <v>0.40453070000000002</v>
       </c>
@@ -7244,15 +7515,24 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U91" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z91" t="e">
+      <c r="U91" s="5">
+        <v>0</v>
+      </c>
+      <c r="V91" s="5">
+        <v>0</v>
+      </c>
+      <c r="W91" s="5">
+        <v>0</v>
+      </c>
+      <c r="X91" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y91">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:25">
       <c r="A92" s="1">
         <v>0.47036689999999998</v>
       </c>
@@ -7317,15 +7597,12 @@
         <f t="shared" si="9"/>
         <v>1.456588</v>
       </c>
-      <c r="U92" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z92" t="e">
+      <c r="Y92" t="e">
         <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:25">
       <c r="A93" s="1">
         <v>0.47586679999999998</v>
       </c>
@@ -7390,15 +7667,24 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U93" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z93" t="e">
+      <c r="U93" s="5">
+        <v>0</v>
+      </c>
+      <c r="V93" s="5">
+        <v>0</v>
+      </c>
+      <c r="W93" s="5">
+        <v>0</v>
+      </c>
+      <c r="X93" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y93">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:25">
       <c r="A94" s="1">
         <v>0.42164439999999997</v>
       </c>
@@ -7463,15 +7749,24 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U94" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z94" t="e">
+      <c r="U94" s="5">
+        <v>0</v>
+      </c>
+      <c r="V94" s="5">
+        <v>0</v>
+      </c>
+      <c r="W94" s="5">
+        <v>0</v>
+      </c>
+      <c r="X94" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y94">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:25">
       <c r="A95" s="1">
         <v>0.45214769999999999</v>
       </c>
@@ -7536,15 +7831,24 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U95" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z95" t="e">
+      <c r="U95" s="5">
+        <v>0</v>
+      </c>
+      <c r="V95" s="5">
+        <v>0</v>
+      </c>
+      <c r="W95" s="5">
+        <v>0</v>
+      </c>
+      <c r="X95" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y95">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:25">
       <c r="A96" s="1">
         <v>0.44742729999999997</v>
       </c>
@@ -7609,15 +7913,24 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U96" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z96" t="e">
+      <c r="U96" s="5">
+        <v>0</v>
+      </c>
+      <c r="V96" s="5">
+        <v>0</v>
+      </c>
+      <c r="W96" s="5">
+        <v>0</v>
+      </c>
+      <c r="X96" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y96">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:25">
       <c r="A97" s="1">
         <v>0.39577839999999997</v>
       </c>
@@ -7682,15 +7995,24 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U97" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z97" t="e">
+      <c r="U97" s="5">
+        <v>0</v>
+      </c>
+      <c r="V97" s="5">
+        <v>0</v>
+      </c>
+      <c r="W97" s="5">
+        <v>0</v>
+      </c>
+      <c r="X97" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y97">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:25">
       <c r="A98" s="1">
         <v>0.55452869999999999</v>
       </c>
@@ -7755,15 +8077,12 @@
         <f t="shared" si="9"/>
         <v>0.68493150000000003</v>
       </c>
-      <c r="U98" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z98" t="e">
+      <c r="Y98" t="e">
         <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:25">
       <c r="A99" s="1">
         <v>0.456621</v>
       </c>
@@ -7828,15 +8147,12 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U99" t="s">
-        <v>102</v>
-      </c>
-      <c r="Z99" t="e">
+      <c r="Y99" t="e">
         <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:25">
       <c r="A100" s="1">
         <v>0.26881719999999998</v>
       </c>
@@ -7901,15 +8217,12 @@
         <f t="shared" si="9"/>
         <v>0.4587156</v>
       </c>
-      <c r="U100" t="s">
-        <v>103</v>
-      </c>
-      <c r="Z100" t="e">
+      <c r="Y100" t="e">
         <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:25">
       <c r="A101" s="1">
         <v>0.3125</v>
       </c>
@@ -7974,15 +8287,12 @@
         <f t="shared" si="9"/>
         <v>0.49019610000000002</v>
       </c>
-      <c r="U101" t="s">
-        <v>104</v>
-      </c>
-      <c r="Z101" t="e">
+      <c r="Y101" t="e">
         <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:25">
       <c r="A102" s="1">
         <v>0.37678980000000001</v>
       </c>
@@ -8047,15 +8357,12 @@
         <f t="shared" si="9"/>
         <v>0.46728969999999997</v>
       </c>
-      <c r="U102" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z102" t="e">
+      <c r="Y102" t="e">
         <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:25">
       <c r="A103" s="1">
         <v>0.43591980000000002</v>
       </c>
@@ -8120,15 +8427,12 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U103" t="s">
-        <v>106</v>
-      </c>
-      <c r="Z103" t="e">
+      <c r="Y103" t="e">
         <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:25">
       <c r="A104" s="1">
         <v>0.54844610000000005</v>
       </c>
@@ -8193,15 +8497,12 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U104" t="s">
-        <v>107</v>
-      </c>
-      <c r="Z104" t="e">
+      <c r="Y104" t="e">
         <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:25">
       <c r="A105" s="1">
         <v>0.24752479999999999</v>
       </c>
@@ -8266,15 +8567,24 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U105" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z105" t="e">
+      <c r="U105" s="5">
+        <v>0</v>
+      </c>
+      <c r="V105" s="5">
+        <v>0</v>
+      </c>
+      <c r="W105" s="5">
+        <v>0</v>
+      </c>
+      <c r="X105" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y105">
         <f t="shared" si="8"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:25">
       <c r="A106" s="1">
         <v>0.3947368</v>
       </c>
@@ -8339,15 +8649,12 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U106" t="s">
-        <v>109</v>
-      </c>
-      <c r="Z106" t="e">
+      <c r="Y106" t="e">
         <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:25">
       <c r="A107" s="1">
         <v>0.41095890000000002</v>
       </c>
@@ -8412,10 +8719,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U107" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z107" t="e">
+      <c r="Y107" t="e">
         <f t="shared" si="8"/>
         <v>#NUM!</v>
       </c>

</xml_diff>